<commit_message>
From rentable to rentform
Now you can choose from the available car list, and direct you to the form, where you will be able to reserve a car.
</commit_message>
<xml_diff>
--- a/CarRentPlanner.xlsx
+++ b/CarRentPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otthon\Documents\GitHub\carrental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A659102A-D1C1-4832-812D-9EA5662DB01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B73D7C-731D-4E38-B736-427E32C4591D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="68">
   <si>
     <t>Honnan (HTML)</t>
   </si>
@@ -227,35 +227,49 @@
     <t>CarDto</t>
   </si>
   <si>
+    <t>Dátumválasztó oldal</t>
+  </si>
+  <si>
+    <t>RentDto</t>
+  </si>
+  <si>
+    <t>/rentform/newrent</t>
+  </si>
+  <si>
     <t>id::int
 name::String
 feePerDay::int
 active::boolean
-picture::?</t>
-  </si>
-  <si>
-    <t>Dátumválasztó oldal</t>
+picture::byte[]</t>
+  </si>
+  <si>
+    <t>carId::Integer
+from:: LocalDate
+to:: LocalDate</t>
   </si>
   <si>
     <t>carId::int
-days::int</t>
-  </si>
-  <si>
-    <t>RentDto</t>
-  </si>
-  <si>
-    <t>/rentform/newrent</t>
+from::LocalDate
+to::LocalDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -367,33 +381,33 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -405,31 +419,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,10 +679,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -685,8 +699,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
@@ -698,8 +712,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="16" t="s">
         <v>43</v>
       </c>
@@ -711,8 +725,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="16" t="s">
         <v>40</v>
       </c>
@@ -724,8 +738,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="16" t="s">
         <v>41</v>
       </c>
@@ -737,14 +751,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -761,8 +775,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
@@ -774,8 +788,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="16" t="s">
         <v>17</v>
       </c>
@@ -787,8 +801,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="19" t="s">
         <v>58</v>
       </c>
@@ -800,8 +814,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="19" t="s">
         <v>59</v>
       </c>
@@ -813,11 +827,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="20" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -834,8 +848,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="21"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="16" t="s">
         <v>45</v>
       </c>
@@ -850,8 +864,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="16" t="s">
         <v>46</v>
       </c>
@@ -866,8 +880,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="21"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="16" t="s">
         <v>47</v>
       </c>
@@ -880,8 +894,8 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="16" t="s">
         <v>48</v>
       </c>
@@ -893,7 +907,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="15"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1878,7 +1892,7 @@
   <dimension ref="A1:G996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1926,7 +1940,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>20</v>
@@ -1939,40 +1953,40 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>34</v>
@@ -1984,13 +1998,13 @@
         <v>35</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1998,7 +2012,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>23</v>
@@ -5088,7 +5102,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5132,16 +5146,16 @@
       <c r="A5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>62</v>
+      <c r="B5" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>